<commit_message>
Charts and tables called race not ethnicity
</commit_message>
<xml_diff>
--- a/data/datasets/housing_and_living_16/access_to_social_housing_measure.xlsx
+++ b/data/datasets/housing_and_living_16/access_to_social_housing_measure.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-21600" yWindow="-22400" windowWidth="21600" windowHeight="38400" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21600" windowHeight="14240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,9 +32,6 @@
     <t>Percentage of groups that live in social housing, rent privately, or own their home</t>
   </si>
   <si>
-    <t>Ethnic group</t>
-  </si>
-  <si>
     <t>Owners</t>
   </si>
   <si>
@@ -42,9 +39,6 @@
   </si>
   <si>
     <t>Private renters</t>
-  </si>
-  <si>
-    <t>Ethnic groups into nine categories</t>
   </si>
   <si>
     <t>White British</t>
@@ -174,6 +168,12 @@
   </si>
   <si>
     <t xml:space="preserve"> 65 or over</t>
+  </si>
+  <si>
+    <t>Race</t>
+  </si>
+  <si>
+    <t>Race groups into nine categories</t>
   </si>
 </sst>
 </file>
@@ -581,9 +581,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -596,9 +593,6 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -610,9 +604,6 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -634,9 +625,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -649,9 +637,6 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -663,9 +648,6 @@
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -685,34 +667,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -732,6 +687,51 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -783,7 +783,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Housing sector for Ethnicity Groups (%age)</a:t>
+              <a:t>Housing sector for Race Groups (%age)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1141,11 +1141,11 @@
         </c:dLbls>
         <c:gapWidth val="53"/>
         <c:overlap val="100"/>
-        <c:axId val="775320864"/>
-        <c:axId val="775322640"/>
+        <c:axId val="2078195536"/>
+        <c:axId val="2131045312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="775320864"/>
+        <c:axId val="2078195536"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1188,7 +1188,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="775322640"/>
+        <c:crossAx val="2131045312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1196,7 +1196,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="775322640"/>
+        <c:axId val="2131045312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -1247,7 +1247,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="775320864"/>
+        <c:crossAx val="2078195536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1618,11 +1618,11 @@
         </c:dLbls>
         <c:gapWidth val="53"/>
         <c:overlap val="100"/>
-        <c:axId val="775555536"/>
-        <c:axId val="775325248"/>
+        <c:axId val="2130861712"/>
+        <c:axId val="2130863760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="775555536"/>
+        <c:axId val="2130861712"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1665,7 +1665,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="775325248"/>
+        <c:crossAx val="2130863760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1673,7 +1673,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="775325248"/>
+        <c:axId val="2130863760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -1724,7 +1724,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="775555536"/>
+        <c:crossAx val="2130861712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1850,7 +1850,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2131,11 +2130,11 @@
         </c:dLbls>
         <c:gapWidth val="53"/>
         <c:overlap val="100"/>
-        <c:axId val="778613808"/>
-        <c:axId val="772250112"/>
+        <c:axId val="2131459184"/>
+        <c:axId val="2131461232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="778613808"/>
+        <c:axId val="2131459184"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2178,7 +2177,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="772250112"/>
+        <c:crossAx val="2131461232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2186,7 +2185,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="772250112"/>
+        <c:axId val="2131461232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -2237,7 +2236,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="778613808"/>
+        <c:crossAx val="2131459184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2251,7 +2250,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2363,7 +2361,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2752,11 +2749,11 @@
         </c:dLbls>
         <c:gapWidth val="53"/>
         <c:overlap val="100"/>
-        <c:axId val="754038432"/>
-        <c:axId val="748794688"/>
+        <c:axId val="2131453184"/>
+        <c:axId val="2131455232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="754038432"/>
+        <c:axId val="2131453184"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2799,7 +2796,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="748794688"/>
+        <c:crossAx val="2131455232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2807,7 +2804,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="748794688"/>
+        <c:axId val="2131455232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -2858,7 +2855,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="754038432"/>
+        <c:crossAx val="2131453184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2872,7 +2869,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2984,7 +2980,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3247,11 +3242,11 @@
         </c:dLbls>
         <c:gapWidth val="53"/>
         <c:overlap val="100"/>
-        <c:axId val="777708512"/>
-        <c:axId val="751477888"/>
+        <c:axId val="2133977792"/>
+        <c:axId val="2133979840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="777708512"/>
+        <c:axId val="2133977792"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3294,7 +3289,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="751477888"/>
+        <c:crossAx val="2133979840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3302,7 +3297,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="751477888"/>
+        <c:axId val="2133979840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -3353,7 +3348,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="777708512"/>
+        <c:crossAx val="2133977792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3367,7 +3362,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6155,7 +6149,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>757341</xdr:colOff>
+      <xdr:colOff>785090</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>144162</xdr:rowOff>
     </xdr:to>
@@ -6572,13 +6566,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F2" zoomScale="165" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="165" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -6591,795 +6585,795 @@
     </row>
     <row r="3" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="E3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="F3" s="39" t="s">
         <v>3</v>
-      </c>
-      <c r="F3" s="54" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="5">
+      <c r="B4" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4">
         <v>67.675927116788458</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>16.562551661401248</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <v>15.761521221810511</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="8"/>
-      <c r="C5" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="10">
+      <c r="B5" s="42"/>
+      <c r="C5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="8">
         <v>35.258252786637676</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="9">
         <v>17.330112427277246</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="10">
         <v>47.411634786085003</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="8"/>
-      <c r="C6" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="10">
+      <c r="B6" s="42"/>
+      <c r="C6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="8">
         <v>29.216008569655997</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="9">
         <v>44.485122215667801</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="10">
         <v>26.298869214676362</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="8"/>
-      <c r="C7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="10">
+      <c r="B7" s="42"/>
+      <c r="C7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="8">
         <v>75.255077656935967</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="9">
         <v>4.7198721896243745</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="10">
         <v>20.025050153439686</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="B8" s="8"/>
-      <c r="C8" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="10">
+      <c r="B8" s="42"/>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="8">
         <v>59.864817020743402</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="9">
         <v>20.468587404854027</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="10">
         <v>19.666595574402532</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="8"/>
-      <c r="C9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="10">
+      <c r="B9" s="42"/>
+      <c r="C9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="8">
         <v>48.297137425213272</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="9">
         <v>13.836769616528438</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="10">
         <v>37.866092958258285</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B10" s="8"/>
-      <c r="C10" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="10">
+      <c r="B10" s="42"/>
+      <c r="C10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="8">
         <v>39.279703577018637</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="9">
         <v>11.21926230500187</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="10">
         <v>49.501034117979557</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="8"/>
-      <c r="C11" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="10">
+      <c r="B11" s="42"/>
+      <c r="C11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="8">
         <v>35.238585092580635</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="9">
         <v>25.397144032155687</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="10">
         <v>39.364270875263678</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="8"/>
-      <c r="C12" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="10">
+      <c r="B12" s="42"/>
+      <c r="C12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="8">
         <v>29.440847655199871</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="9">
         <v>24.049378047146835</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="10">
         <v>46.509774297653294</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="13"/>
-      <c r="C13" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="15">
+      <c r="B13" s="43"/>
+      <c r="C13" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="12">
         <v>63.613761826510675</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="13">
         <v>17.373602604960031</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="14">
         <v>19.012635568529014</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>16</v>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="50" t="s">
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="53" t="s">
+      <c r="F16" s="39" t="s">
         <v>3</v>
-      </c>
-      <c r="F16" s="54" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="B17" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="24">
+      <c r="B17" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="20">
         <v>24.302173984934392</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="21">
         <v>13.242699688992879</v>
       </c>
-      <c r="F17" s="26">
+      <c r="F17" s="22">
         <v>62.455126326072644</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="27"/>
-      <c r="C18" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="29">
+      <c r="B18" s="45"/>
+      <c r="C18" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="24">
         <v>66.48623525643427</v>
       </c>
-      <c r="E18" s="30">
+      <c r="E18" s="25">
         <v>17.417329300143905</v>
       </c>
-      <c r="F18" s="31">
+      <c r="F18" s="26">
         <v>16.096435443421637</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="27"/>
-      <c r="C19" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="29">
+      <c r="B19" s="45"/>
+      <c r="C19" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="24">
         <v>34.679349933721149</v>
       </c>
-      <c r="E19" s="30">
+      <c r="E19" s="25">
         <v>19.501635449267408</v>
       </c>
-      <c r="F19" s="31">
+      <c r="F19" s="26">
         <v>45.819014617011476</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="32"/>
-      <c r="C20" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="34">
+      <c r="B20" s="46"/>
+      <c r="C20" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="28">
         <v>63.643950196591383</v>
       </c>
-      <c r="E20" s="35">
+      <c r="E20" s="29">
         <v>17.336036169374875</v>
       </c>
-      <c r="F20" s="36">
+      <c r="F20" s="30">
         <v>19.020013634033432</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>16</v>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B22" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="21" t="s">
-        <v>16</v>
+      <c r="B22" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="38" t="s">
-        <v>16</v>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="32" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="21"/>
-      <c r="C24" s="49" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="50" t="s">
+      <c r="B24" s="18"/>
+      <c r="C24" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E24" s="51" t="s">
+      <c r="F24" s="37" t="s">
         <v>3</v>
-      </c>
-      <c r="F24" s="52" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="B25" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="24">
+      <c r="B25" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="20">
         <v>47.219631308167337</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="21">
         <v>29.996578819192983</v>
       </c>
-      <c r="F25" s="26">
+      <c r="F25" s="22">
         <v>22.783789872639318</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B26" s="40"/>
-      <c r="C26" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="29">
+      <c r="B26" s="48"/>
+      <c r="C26" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="24">
         <v>50.087528667033745</v>
       </c>
-      <c r="E26" s="30">
+      <c r="E26" s="25">
         <v>29.284244011198684</v>
       </c>
-      <c r="F26" s="31">
+      <c r="F26" s="26">
         <v>20.628227321767465</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B27" s="40"/>
-      <c r="C27" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="29">
+      <c r="B27" s="48"/>
+      <c r="C27" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="24">
         <v>61.647819647546733</v>
       </c>
-      <c r="E27" s="30">
+      <c r="E27" s="25">
         <v>17.726820907982923</v>
       </c>
-      <c r="F27" s="31">
+      <c r="F27" s="26">
         <v>20.625359444470217</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B28" s="40"/>
-      <c r="C28" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" s="29">
+      <c r="B28" s="48"/>
+      <c r="C28" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="24">
         <v>73.373845494702593</v>
       </c>
-      <c r="E28" s="30">
+      <c r="E28" s="25">
         <v>8.2046680849731484</v>
       </c>
-      <c r="F28" s="31">
+      <c r="F28" s="26">
         <v>18.421486420323987</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="B29" s="40"/>
-      <c r="C29" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="29">
+      <c r="B29" s="48"/>
+      <c r="C29" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="24">
         <v>84.929535107834212</v>
       </c>
-      <c r="E29" s="30">
+      <c r="E29" s="25">
         <v>2.2872948143706187</v>
       </c>
-      <c r="F29" s="31">
+      <c r="F29" s="26">
         <v>12.783170077795262</v>
       </c>
     </row>
     <row r="30" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="41"/>
-      <c r="C30" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30" s="34">
+      <c r="B30" s="49"/>
+      <c r="C30" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="28">
         <v>63.621957628165084</v>
       </c>
-      <c r="E30" s="35">
+      <c r="E30" s="29">
         <v>17.374843132523665</v>
       </c>
-      <c r="F30" s="36">
+      <c r="F30" s="30">
         <v>19.003199239310938</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F31" s="18" t="s">
-        <v>16</v>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B32" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E32" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32" s="21" t="s">
-        <v>16</v>
+      <c r="B32" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="F33" s="38" t="s">
-        <v>16</v>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="32" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="21"/>
-      <c r="C34" s="49" t="s">
-        <v>30</v>
-      </c>
-      <c r="D34" s="50" t="s">
+      <c r="B34" s="18"/>
+      <c r="C34" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="51" t="s">
+      <c r="F34" s="37" t="s">
         <v>3</v>
-      </c>
-      <c r="F34" s="52" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B35" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="D35" s="24">
+      <c r="B35" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" s="20">
         <v>60.827178271023222</v>
       </c>
-      <c r="E35" s="25">
+      <c r="E35" s="21">
         <v>22.981683055475436</v>
       </c>
-      <c r="F35" s="26">
+      <c r="F35" s="22">
         <v>16.191138673501325</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B36" s="43"/>
-      <c r="C36" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="D36" s="29">
+      <c r="B36" s="51"/>
+      <c r="C36" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" s="24">
         <v>64.721629526299907</v>
       </c>
-      <c r="E36" s="30">
+      <c r="E36" s="25">
         <v>18.143047912938648</v>
       </c>
-      <c r="F36" s="31">
+      <c r="F36" s="26">
         <v>17.135322560761498</v>
       </c>
     </row>
     <row r="37" spans="2:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="B37" s="43"/>
-      <c r="C37" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="D37" s="29">
+      <c r="B37" s="51"/>
+      <c r="C37" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="24">
         <v>62.59964929355003</v>
       </c>
-      <c r="E37" s="30">
+      <c r="E37" s="25">
         <v>18.181390683625192</v>
       </c>
-      <c r="F37" s="31">
+      <c r="F37" s="26">
         <v>19.218960022824721</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B38" s="43"/>
-      <c r="C38" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="D38" s="29">
+      <c r="B38" s="51"/>
+      <c r="C38" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D38" s="24">
         <v>66.589312542696987</v>
       </c>
-      <c r="E38" s="30">
+      <c r="E38" s="25">
         <v>15.879532561560742</v>
       </c>
-      <c r="F38" s="31">
+      <c r="F38" s="26">
         <v>17.531154895742262</v>
       </c>
     </row>
-    <row r="39" spans="2:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="B39" s="43"/>
-      <c r="C39" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="D39" s="29">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B39" s="51"/>
+      <c r="C39" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="24">
         <v>65.776165303450242</v>
       </c>
-      <c r="E39" s="30">
+      <c r="E39" s="25">
         <v>18.579135187082134</v>
       </c>
-      <c r="F39" s="31">
+      <c r="F39" s="26">
         <v>15.644699509467774</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B40" s="43"/>
-      <c r="C40" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="D40" s="29">
+      <c r="B40" s="51"/>
+      <c r="C40" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" s="24">
         <v>67.096225933447315</v>
       </c>
-      <c r="E40" s="30">
+      <c r="E40" s="25">
         <v>15.650764925671268</v>
       </c>
-      <c r="F40" s="31">
+      <c r="F40" s="26">
         <v>17.253009140881396</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="43"/>
-      <c r="C41" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="D41" s="29">
+      <c r="B41" s="51"/>
+      <c r="C41" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" s="24">
         <v>49.536088406859079</v>
       </c>
-      <c r="E41" s="30">
+      <c r="E41" s="25">
         <v>23.264486855471198</v>
       </c>
-      <c r="F41" s="31">
+      <c r="F41" s="26">
         <v>27.199424737669876</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B42" s="43"/>
-      <c r="C42" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="D42" s="29">
+      <c r="B42" s="51"/>
+      <c r="C42" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" s="24">
         <v>68.063189308328674</v>
       </c>
-      <c r="E42" s="30">
+      <c r="E42" s="25">
         <v>13.12840711520832</v>
       </c>
-      <c r="F42" s="31">
+      <c r="F42" s="26">
         <v>18.808403576463036</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B43" s="43"/>
-      <c r="C43" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="D43" s="29">
+      <c r="B43" s="51"/>
+      <c r="C43" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D43" s="24">
         <v>69.086714670687272</v>
       </c>
-      <c r="E43" s="30">
+      <c r="E43" s="25">
         <v>13.14979029735478</v>
       </c>
-      <c r="F43" s="31">
+      <c r="F43" s="26">
         <v>17.763495031957881</v>
       </c>
     </row>
-    <row r="44" spans="2:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="B44" s="43"/>
-      <c r="C44" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="D44" s="29">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B44" s="51"/>
+      <c r="C44" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44" s="24">
         <v>0</v>
       </c>
-      <c r="E44" s="30">
+      <c r="E44" s="25">
         <v>0</v>
       </c>
-      <c r="F44" s="31">
+      <c r="F44" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B45" s="43"/>
-      <c r="C45" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="D45" s="29">
+      <c r="B45" s="51"/>
+      <c r="C45" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D45" s="24">
         <v>0</v>
       </c>
-      <c r="E45" s="30">
+      <c r="E45" s="25">
         <v>0</v>
       </c>
-      <c r="F45" s="31">
+      <c r="F45" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="44"/>
-      <c r="C46" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D46" s="34">
+      <c r="B46" s="52"/>
+      <c r="C46" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" s="28">
         <v>63.621957628165084</v>
       </c>
-      <c r="E46" s="35">
+      <c r="E46" s="29">
         <v>17.374843132523665</v>
       </c>
-      <c r="F46" s="36">
+      <c r="F46" s="30">
         <v>19.003199239310938</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B47" s="45"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="E47" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="F47" s="45" t="s">
-        <v>16</v>
+      <c r="B47" s="33"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E47" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" s="33" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B48" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E48" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F48" s="21" t="s">
-        <v>16</v>
+      <c r="B48" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E48" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F48" s="18" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="E49" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="F49" s="38" t="s">
-        <v>16</v>
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="E49" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F49" s="32" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="21"/>
-      <c r="C50" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="D50" s="50" t="s">
+      <c r="B50" s="18"/>
+      <c r="C50" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D50" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="E50" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E50" s="51" t="s">
+      <c r="F50" s="37" t="s">
         <v>3</v>
-      </c>
-      <c r="F50" s="52" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B51" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="C51" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="D51" s="24">
+      <c r="B51" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D51" s="20">
         <v>21.04647154329135</v>
       </c>
-      <c r="E51" s="25">
+      <c r="E51" s="21">
         <v>18.996686061765665</v>
       </c>
-      <c r="F51" s="26">
+      <c r="F51" s="22">
         <v>59.956842394942974</v>
       </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B52" s="47"/>
-      <c r="C52" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="D52" s="29">
+      <c r="B52" s="54"/>
+      <c r="C52" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D52" s="24">
         <v>54.165833114943197</v>
       </c>
-      <c r="E52" s="30">
+      <c r="E52" s="25">
         <v>17.18501935414459</v>
       </c>
-      <c r="F52" s="31">
+      <c r="F52" s="26">
         <v>28.649147530912145</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B53" s="47"/>
-      <c r="C53" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="D53" s="29">
+      <c r="B53" s="54"/>
+      <c r="C53" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D53" s="24">
         <v>71.762068578853004</v>
       </c>
-      <c r="E53" s="30">
+      <c r="E53" s="25">
         <v>16.912822349319935</v>
       </c>
-      <c r="F53" s="31">
+      <c r="F53" s="26">
         <v>11.325109071827235</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B54" s="47"/>
-      <c r="C54" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="D54" s="29">
+      <c r="B54" s="54"/>
+      <c r="C54" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D54" s="24">
         <v>76.742786956268688</v>
       </c>
-      <c r="E54" s="30">
+      <c r="E54" s="25">
         <v>17.564339130594686</v>
       </c>
-      <c r="F54" s="31">
+      <c r="F54" s="26">
         <v>5.6928739131365642</v>
       </c>
     </row>
     <row r="55" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="48"/>
-      <c r="C55" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D55" s="34">
+      <c r="B55" s="55"/>
+      <c r="C55" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" s="28">
         <v>63.621957628165084</v>
       </c>
-      <c r="E55" s="35">
+      <c r="E55" s="29">
         <v>17.374843132523665</v>
       </c>
-      <c r="F55" s="36">
+      <c r="F55" s="30">
         <v>19.003199239310938</v>
       </c>
     </row>
     <row r="68" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K68" s="55"/>
+      <c r="K68" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>